<commit_message>
Check date handling in tests
</commit_message>
<xml_diff>
--- a/tests/sources/people.xlsx
+++ b/tests/sources/people.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inxilpro/Development/open-source/conveyor-belt/tests/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB042A84-E3FA-FA4E-8167-96632CCE0119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0729CC3-BA74-2948-AB4A-041BD95A2D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27880" yWindow="7420" windowWidth="28040" windowHeight="17440" xr2:uid="{D1244214-251E-6C4F-9FF9-1584D431553B}"/>
+    <workbookView xWindow="6440" yWindow="6240" windowWidth="28040" windowHeight="17440" xr2:uid="{D1244214-251E-6C4F-9FF9-1584D431553B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Company</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Galahad, Inc.</t>
+  </si>
+  <si>
+    <t>Quoted At</t>
   </si>
 </sst>
 </file>
@@ -113,9 +116,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A927DFC4-571F-5543-8089-D3C874017084}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -441,9 +446,10 @@
     <col min="1" max="1" width="18.6640625" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" customWidth="1"/>
     <col min="3" max="3" width="44.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -453,8 +459,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -464,8 +473,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
+      <c r="D2" s="3">
+        <v>44197</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -475,8 +487,11 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
+      <c r="D3" s="3">
+        <v>43845</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -484,7 +499,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -493,6 +508,9 @@
       </c>
       <c r="C5" t="s">
         <v>9</v>
+      </c>
+      <c r="D5" s="3">
+        <v>43528</v>
       </c>
     </row>
   </sheetData>

</xml_diff>